<commit_message>
Adding new jupyter notebooks
</commit_message>
<xml_diff>
--- a/my1.xlsx
+++ b/my1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5706FA77-1880-42A6-B4DF-D7A48CA40EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C358D7-32D5-4054-902E-9AD71CC59E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD9D5D98-5DBD-483B-BACF-825341D464F4}"/>
+    <workbookView xWindow="3660" yWindow="3660" windowWidth="17280" windowHeight="8880" xr2:uid="{AD9D5D98-5DBD-483B-BACF-825341D464F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,25 +569,16 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
@@ -607,9 +598,6 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
       <c r="D4">
         <v>1</v>
       </c>
@@ -686,9 +674,6 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -715,9 +700,6 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -729,9 +711,6 @@
       </c>
       <c r="H7">
         <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -835,9 +814,6 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
       <c r="J10">
         <v>1</v>
       </c>
@@ -852,14 +828,8 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
         <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>

</xml_diff>